<commit_message>
added shuffle to the sudoku puzzle generator
</commit_message>
<xml_diff>
--- a/Distribution/Sudoku.xlsx
+++ b/Distribution/Sudoku.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\ACQ\ACQ.Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\ACQ\Distribution\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -560,7 +560,7 @@
   <dimension ref="B2:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,54 +603,54 @@
       <c r="C4" s="2" t="str">
         <v/>
       </c>
-      <c r="D4" s="3" t="str">
-        <v/>
+      <c r="D4" s="3">
+        <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2" t="str">
         <v/>
       </c>
-      <c r="G4" s="3">
-        <v>1</v>
+      <c r="G4" s="3" t="str">
+        <v/>
       </c>
       <c r="H4" s="1" t="str">
         <v/>
       </c>
-      <c r="I4" s="2">
-        <v>9</v>
-      </c>
-      <c r="J4" s="3" t="str">
-        <v/>
+      <c r="I4" s="2" t="str">
+        <v/>
+      </c>
+      <c r="J4" s="3">
+        <v>8</v>
       </c>
       <c r="L4" s="1">
         <f t="array" ref="L4:T12">_xll.acq_sudoku_solve(B4:J12)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M4" s="2">
         <v>4</v>
       </c>
       <c r="N4" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="O4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P4" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="Q4" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="R4" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S4" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="T4" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="V4" t="s">
         <v>3</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="5" t="str">
         <v/>
@@ -671,60 +671,60 @@
         <v/>
       </c>
       <c r="E5" s="4">
-        <v>6</v>
-      </c>
-      <c r="F5" s="5" t="str">
-        <v/>
+        <v>4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>9</v>
       </c>
       <c r="G5" s="6" t="str">
         <v/>
       </c>
-      <c r="H5" s="4">
-        <v>1</v>
+      <c r="H5" s="4" t="str">
+        <v/>
       </c>
       <c r="I5" s="5" t="str">
         <v/>
       </c>
-      <c r="J5" s="6" t="str">
-        <v/>
+      <c r="J5" s="6">
+        <v>2</v>
       </c>
       <c r="L5" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="M5" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N5" s="6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O5" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P5" s="5">
         <v>9</v>
       </c>
       <c r="Q5" s="6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="R5" s="4">
         <v>1</v>
       </c>
       <c r="S5" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T5" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="7" t="str">
         <v/>
       </c>
-      <c r="C6" s="8" t="str">
-        <v/>
+      <c r="C6" s="8">
+        <v>3</v>
       </c>
       <c r="D6" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="7" t="str">
         <v/>
@@ -742,34 +742,34 @@
         <v/>
       </c>
       <c r="J6" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L6" s="7">
         <v>2</v>
       </c>
       <c r="M6" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N6" s="9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O6" s="7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P6" s="8">
         <v>5</v>
       </c>
       <c r="Q6" s="9">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="R6" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S6" s="8">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="T6" s="9">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.35">
@@ -783,7 +783,7 @@
         <v/>
       </c>
       <c r="E7" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2" t="str">
         <v/>
@@ -791,97 +791,97 @@
       <c r="G7" s="3" t="str">
         <v/>
       </c>
-      <c r="H7" s="1" t="str">
-        <v/>
-      </c>
-      <c r="I7" s="2">
-        <v>3</v>
-      </c>
-      <c r="J7" s="3" t="str">
-        <v/>
+      <c r="H7" s="1">
+        <v>9</v>
+      </c>
+      <c r="I7" s="2" t="str">
+        <v/>
+      </c>
+      <c r="J7" s="3">
+        <v>6</v>
       </c>
       <c r="L7" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M7" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N7" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="P7" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="Q7" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R7" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="S7" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T7" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="B8" s="4" t="str">
-        <v/>
+      <c r="B8" s="4">
+        <v>1</v>
       </c>
       <c r="C8" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D8" s="6">
-        <v>4</v>
-      </c>
-      <c r="E8" s="4">
-        <v>2</v>
-      </c>
-      <c r="F8" s="5" t="str">
-        <v/>
-      </c>
-      <c r="G8" s="6">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="E8" s="4" t="str">
+        <v/>
+      </c>
+      <c r="F8" s="5">
+        <v>7</v>
+      </c>
+      <c r="G8" s="6" t="str">
+        <v/>
       </c>
       <c r="H8" s="4" t="str">
         <v/>
       </c>
-      <c r="I8" s="5" t="str">
-        <v/>
+      <c r="I8" s="5">
+        <v>8</v>
       </c>
       <c r="J8" s="6" t="str">
         <v/>
       </c>
       <c r="L8" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M8" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="N8" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O8" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P8" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="Q8" s="6">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="R8" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="S8" s="5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="T8" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -891,8 +891,8 @@
       <c r="C9" s="8" t="str">
         <v/>
       </c>
-      <c r="D9" s="9">
-        <v>5</v>
+      <c r="D9" s="9" t="str">
+        <v/>
       </c>
       <c r="E9" s="7" t="str">
         <v/>
@@ -900,8 +900,8 @@
       <c r="F9" s="8" t="str">
         <v/>
       </c>
-      <c r="G9" s="9">
-        <v>9</v>
+      <c r="G9" s="9" t="str">
+        <v/>
       </c>
       <c r="H9" s="7" t="str">
         <v/>
@@ -909,23 +909,23 @@
       <c r="I9" s="8" t="str">
         <v/>
       </c>
-      <c r="J9" s="9">
-        <v>6</v>
+      <c r="J9" s="9" t="str">
+        <v/>
       </c>
       <c r="L9" s="7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M9" s="8">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N9" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O9" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P9" s="8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Q9" s="9">
         <v>9</v>
@@ -934,15 +934,15 @@
         <v>7</v>
       </c>
       <c r="S9" s="8">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="T9" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="B10" s="1" t="str">
-        <v/>
+      <c r="B10" s="1">
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="str">
         <v/>
@@ -950,64 +950,64 @@
       <c r="D10" s="3" t="str">
         <v/>
       </c>
-      <c r="E10" s="1">
-        <v>5</v>
+      <c r="E10" s="1" t="str">
+        <v/>
       </c>
       <c r="F10" s="2" t="str">
         <v/>
       </c>
-      <c r="G10" s="3" t="str">
-        <v/>
+      <c r="G10" s="3">
+        <v>5</v>
       </c>
       <c r="H10" s="1" t="str">
         <v/>
       </c>
-      <c r="I10" s="2" t="str">
-        <v/>
-      </c>
-      <c r="J10" s="3" t="str">
-        <v/>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>3</v>
       </c>
       <c r="L10" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M10" s="2">
         <v>8</v>
       </c>
       <c r="N10" s="3">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="O10" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P10" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Q10" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R10" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="S10" s="2">
         <v>1</v>
       </c>
       <c r="T10" s="3">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="str">
         <v/>
       </c>
-      <c r="C11" s="5">
-        <v>6</v>
+      <c r="C11" s="5" t="str">
+        <v/>
       </c>
       <c r="D11" s="6" t="str">
         <v/>
       </c>
-      <c r="E11" s="4" t="str">
-        <v/>
+      <c r="E11" s="4">
+        <v>9</v>
       </c>
       <c r="F11" s="5" t="str">
         <v/>
@@ -1018,46 +1018,46 @@
       <c r="H11" s="4" t="str">
         <v/>
       </c>
-      <c r="I11" s="5">
-        <v>7</v>
-      </c>
-      <c r="J11" s="6">
-        <v>3</v>
+      <c r="I11" s="5" t="str">
+        <v/>
+      </c>
+      <c r="J11" s="6" t="str">
+        <v/>
       </c>
       <c r="L11" s="4">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="M11" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="N11" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O11" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P11" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="R11" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="S11" s="5">
         <v>7</v>
       </c>
       <c r="T11" s="6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="7" t="str">
         <v/>
       </c>
-      <c r="C12" s="8" t="str">
-        <v/>
+      <c r="C12" s="8">
+        <v>2</v>
       </c>
       <c r="D12" s="9" t="str">
         <v/>
@@ -1065,14 +1065,14 @@
       <c r="E12" s="7" t="str">
         <v/>
       </c>
-      <c r="F12" s="8">
-        <v>7</v>
+      <c r="F12" s="8" t="str">
+        <v/>
       </c>
       <c r="G12" s="9" t="str">
         <v/>
       </c>
       <c r="H12" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I12" s="8" t="str">
         <v/>
@@ -1081,31 +1081,31 @@
         <v/>
       </c>
       <c r="L12" s="7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M12" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N12" s="9">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O12" s="7">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="P12" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q12" s="9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="R12" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="S12" s="8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T12" s="9">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.35">
@@ -1177,57 +1177,57 @@
         <f t="array" ref="B16:J24">_xll.acq_sudoku_generate(W17)</f>
         <v/>
       </c>
-      <c r="C16" s="2" t="str">
-        <v/>
-      </c>
-      <c r="D16" s="3" t="str">
-        <v/>
+      <c r="C16" s="2">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3">
+        <v>4</v>
       </c>
       <c r="E16" s="1" t="str">
         <v/>
       </c>
-      <c r="F16" s="2">
-        <v>7</v>
-      </c>
-      <c r="G16" s="3" t="str">
-        <v/>
-      </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2" t="str">
-        <v/>
+      <c r="F16" s="2" t="str">
+        <v/>
+      </c>
+      <c r="G16" s="3">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1" t="str">
+        <v/>
+      </c>
+      <c r="I16" s="2">
+        <v>5</v>
       </c>
       <c r="J16" s="3" t="str">
         <v/>
       </c>
       <c r="L16" s="1">
         <f t="array" ref="L16:T24">_xll.acq_sudoku_solve(B16:J24)</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M16" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N16" s="3">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="O16" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P16" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="R16" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S16" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="T16" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V16" t="s">
         <v>3</v>
@@ -1241,56 +1241,56 @@
       <c r="B17" s="4" t="str">
         <v/>
       </c>
-      <c r="C17" s="5">
-        <v>7</v>
-      </c>
-      <c r="D17" s="6" t="str">
-        <v/>
-      </c>
-      <c r="E17" s="4" t="str">
-        <v/>
+      <c r="C17" s="5" t="str">
+        <v/>
+      </c>
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4">
+        <v>6</v>
       </c>
       <c r="F17" s="5" t="str">
         <v/>
       </c>
-      <c r="G17" s="6" t="str">
-        <v/>
+      <c r="G17" s="6">
+        <v>7</v>
       </c>
       <c r="H17" s="4" t="str">
         <v/>
       </c>
-      <c r="I17" s="5">
-        <v>5</v>
+      <c r="I17" s="5" t="str">
+        <v/>
       </c>
       <c r="J17" s="6">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="L17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M17" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N17" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O17" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P17" s="5">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q17" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R17" s="4">
         <v>3</v>
       </c>
       <c r="S17" s="5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="T17" s="6">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="V17" t="s">
         <v>7</v>
@@ -1306,17 +1306,17 @@
       <c r="C18" s="8" t="str">
         <v/>
       </c>
-      <c r="D18" s="9">
-        <v>4</v>
-      </c>
-      <c r="E18" s="7">
-        <v>3</v>
+      <c r="D18" s="9" t="str">
+        <v/>
+      </c>
+      <c r="E18" s="7" t="str">
+        <v/>
       </c>
       <c r="F18" s="8" t="str">
         <v/>
       </c>
-      <c r="G18" s="9">
-        <v>9</v>
+      <c r="G18" s="9" t="str">
+        <v/>
       </c>
       <c r="H18" s="7" t="str">
         <v/>
@@ -1328,95 +1328,95 @@
         <v/>
       </c>
       <c r="L18" s="7">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M18" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N18" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O18" s="7">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="P18" s="8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q18" s="9">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="R18" s="7">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="S18" s="8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="T18" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="str">
         <v/>
       </c>
-      <c r="C19" s="2">
-        <v>3</v>
-      </c>
-      <c r="D19" s="3">
-        <v>7</v>
+      <c r="C19" s="2" t="str">
+        <v/>
+      </c>
+      <c r="D19" s="3" t="str">
+        <v/>
       </c>
       <c r="E19" s="1" t="str">
         <v/>
       </c>
-      <c r="F19" s="2">
-        <v>5</v>
+      <c r="F19" s="2" t="str">
+        <v/>
       </c>
       <c r="G19" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H19" s="1" t="str">
         <v/>
       </c>
-      <c r="I19" s="2">
-        <v>4</v>
+      <c r="I19" s="2" t="str">
+        <v/>
       </c>
       <c r="J19" s="3" t="str">
         <v/>
       </c>
       <c r="L19" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M19" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N19" s="3">
         <v>7</v>
       </c>
       <c r="O19" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="P19" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Q19" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="R19" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="S19" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T19" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="B20" s="4" t="str">
-        <v/>
+      <c r="B20" s="4">
+        <v>8</v>
       </c>
       <c r="C20" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D20" s="6" t="str">
         <v/>
@@ -1424,11 +1424,11 @@
       <c r="E20" s="4" t="str">
         <v/>
       </c>
-      <c r="F20" s="5">
-        <v>3</v>
-      </c>
-      <c r="G20" s="6" t="str">
-        <v/>
+      <c r="F20" s="5" t="str">
+        <v/>
+      </c>
+      <c r="G20" s="6">
+        <v>3</v>
       </c>
       <c r="H20" s="4" t="str">
         <v/>
@@ -1437,48 +1437,48 @@
         <v/>
       </c>
       <c r="J20" s="6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L20" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M20" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N20" s="6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O20" s="4">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P20" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q20" s="6">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="R20" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S20" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="T20" s="6">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="7" t="str">
         <v/>
       </c>
-      <c r="C21" s="8">
-        <v>9</v>
+      <c r="C21" s="8" t="str">
+        <v/>
       </c>
       <c r="D21" s="9" t="str">
         <v/>
       </c>
       <c r="E21" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F21" s="8" t="str">
         <v/>
@@ -1487,7 +1487,7 @@
         <v/>
       </c>
       <c r="H21" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I21" s="8" t="str">
         <v/>
@@ -1496,39 +1496,39 @@
         <v/>
       </c>
       <c r="L21" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M21" s="8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N21" s="9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O21" s="7">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="P21" s="8">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q21" s="9">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="R21" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S21" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T21" s="9">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="str">
         <v/>
       </c>
-      <c r="C22" s="2" t="str">
-        <v/>
+      <c r="C22" s="2">
+        <v>1</v>
       </c>
       <c r="D22" s="3" t="str">
         <v/>
@@ -1542,41 +1542,41 @@
       <c r="G22" s="3" t="str">
         <v/>
       </c>
-      <c r="H22" s="1">
-        <v>2</v>
+      <c r="H22" s="1" t="str">
+        <v/>
       </c>
       <c r="I22" s="2" t="str">
         <v/>
       </c>
-      <c r="J22" s="3">
-        <v>5</v>
+      <c r="J22" s="3" t="str">
+        <v/>
       </c>
       <c r="L22" s="1">
         <v>9</v>
       </c>
       <c r="M22" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N22" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="O22" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P22" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="Q22" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R22" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="S22" s="2">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="T22" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.35">
@@ -1586,109 +1586,109 @@
       <c r="C23" s="5" t="str">
         <v/>
       </c>
-      <c r="D23" s="6" t="str">
-        <v/>
+      <c r="D23" s="6">
+        <v>6</v>
       </c>
       <c r="E23" s="4" t="str">
         <v/>
       </c>
-      <c r="F23" s="5" t="str">
-        <v/>
-      </c>
-      <c r="G23" s="6" t="str">
-        <v/>
-      </c>
-      <c r="H23" s="4" t="str">
-        <v/>
-      </c>
-      <c r="I23" s="5">
-        <v>1</v>
+      <c r="F23" s="5">
+        <v>3</v>
+      </c>
+      <c r="G23" s="6">
+        <v>5</v>
+      </c>
+      <c r="H23" s="4">
+        <v>9</v>
+      </c>
+      <c r="I23" s="5" t="str">
+        <v/>
       </c>
       <c r="J23" s="6" t="str">
         <v/>
       </c>
       <c r="L23" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="M23" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="N23" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O23" s="4">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="P23" s="5">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="Q23" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R23" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S23" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T23" s="6">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="7">
-        <v>6</v>
+      <c r="B24" s="7" t="str">
+        <v/>
       </c>
       <c r="C24" s="8" t="str">
         <v/>
       </c>
       <c r="D24" s="9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E24" s="7" t="str">
         <v/>
       </c>
-      <c r="F24" s="8">
-        <v>2</v>
+      <c r="F24" s="8" t="str">
+        <v/>
       </c>
       <c r="G24" s="9" t="str">
         <v/>
       </c>
-      <c r="H24" s="7">
-        <v>4</v>
-      </c>
-      <c r="I24" s="8" t="str">
-        <v/>
+      <c r="H24" s="7" t="str">
+        <v/>
+      </c>
+      <c r="I24" s="8">
+        <v>8</v>
       </c>
       <c r="J24" s="9" t="str">
         <v/>
       </c>
       <c r="L24" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M24" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="N24" s="9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O24" s="7">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="P24" s="8">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="Q24" s="9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R24" s="7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S24" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="T24" s="9">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>